<commit_message>
Planning aangepast, alle BB documenten toegevoegd.
</commit_message>
<xml_diff>
--- a/Documentatie/Planning + Taakverdeling.xlsx
+++ b/Documentatie/Planning + Taakverdeling.xlsx
@@ -199,9 +199,6 @@
     <t>Analyse 1 (Do)</t>
   </si>
   <si>
-    <t>&lt;&lt; deze rij moet mis onder kopje docu</t>
-  </si>
-  <si>
     <t>Inleveren kleur anders?</t>
   </si>
   <si>
@@ -215,6 +212,9 @@
   </si>
   <si>
     <t>Joshua, Remco, Melinda, Arjen, Jeffrey en Yme</t>
+  </si>
+  <si>
+    <t>&lt;&lt; zie verslag_onderdelen.doc</t>
   </si>
 </sst>
 </file>
@@ -450,42 +450,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -526,32 +490,68 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -873,28 +873,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47:O47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="18" t="s">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -905,62 +905,62 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="19" t="s">
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="19"/>
+      <c r="G4" s="38"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="28">
+      <c r="F5" s="16">
         <v>46</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="17">
         <v>47</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="18">
         <v>48</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="19">
         <v>49</v>
       </c>
-      <c r="J5" s="32">
+      <c r="J5" s="20">
         <v>50</v>
       </c>
-      <c r="K5" s="33">
+      <c r="K5" s="21">
         <v>51</v>
       </c>
-      <c r="L5" s="34">
+      <c r="L5" s="22">
         <v>52</v>
       </c>
-      <c r="M5" s="35">
+      <c r="M5" s="23">
         <v>1</v>
       </c>
-      <c r="N5" s="36">
+      <c r="N5" s="24">
         <v>2</v>
       </c>
-      <c r="O5" s="37">
+      <c r="O5" s="25">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
       <c r="E6" s="2"/>
       <c r="F6" s="3"/>
       <c r="G6" s="2"/>
@@ -968,440 +968,437 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="52" t="s">
+      <c r="L6" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="52"/>
+      <c r="M6" s="51"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="38"/>
+      <c r="F7" s="26"/>
       <c r="G7" s="3"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="52"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="51"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="38"/>
+      <c r="F8" s="26"/>
       <c r="G8" s="2"/>
       <c r="H8" s="3"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="52"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="38"/>
+      <c r="F9" s="26"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="3"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="51"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="38"/>
+      <c r="F10" s="26"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="3"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="52"/>
-      <c r="M10" s="52"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="38"/>
+      <c r="F11" s="26"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="3"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="38"/>
+      <c r="F12" s="26"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="S12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="38"/>
+      <c r="F13" s="26"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="52"/>
+      <c r="L13" s="51"/>
+      <c r="M13" s="51"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="38"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="52"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="51"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="49" t="s">
+      <c r="A15" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="47"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="54"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="38"/>
+      <c r="F15" s="26"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="52"/>
-      <c r="M15" s="52"/>
+      <c r="L15" s="51"/>
+      <c r="M15" s="51"/>
       <c r="N15" s="3"/>
       <c r="O15" s="2"/>
-      <c r="Q15" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="38"/>
+      <c r="F16" s="26"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-      <c r="L16" s="52"/>
-      <c r="M16" s="52"/>
+      <c r="L16" s="51"/>
+      <c r="M16" s="51"/>
       <c r="N16" s="2"/>
       <c r="O16" s="3"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="38"/>
+      <c r="F17" s="26"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="52"/>
-      <c r="M17" s="52"/>
+      <c r="L17" s="51"/>
+      <c r="M17" s="51"/>
       <c r="N17" s="2"/>
       <c r="O17" s="3"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="27"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="42"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="38"/>
+      <c r="F18" s="26"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="52"/>
-      <c r="M18" s="52"/>
+      <c r="L18" s="51"/>
+      <c r="M18" s="51"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="27"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="42"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="38"/>
+      <c r="F19" s="26"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="4"/>
       <c r="K19" s="9"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="52"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="52"/>
-      <c r="M20" s="52"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
+      <c r="A21" s="36"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="52"/>
-      <c r="M21" s="52"/>
-      <c r="N21" s="44"/>
-      <c r="O21" s="44"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="27"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="42"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="52"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="45"/>
-      <c r="O22" s="45"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="51"/>
+      <c r="M22" s="51"/>
+      <c r="N22" s="33"/>
+      <c r="O22" s="33"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="10"/>
       <c r="K23" s="11"/>
-      <c r="L23" s="52"/>
-      <c r="M23" s="52"/>
+      <c r="L23" s="51"/>
+      <c r="M23" s="51"/>
       <c r="N23" s="12"/>
       <c r="O23" s="12"/>
       <c r="S23" t="s">
         <v>14</v>
       </c>
       <c r="U23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
+      <c r="A24" s="36"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="44"/>
-      <c r="K24" s="44"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="52"/>
-      <c r="N24" s="45"/>
-      <c r="O24" s="45"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="51"/>
+      <c r="M24" s="51"/>
+      <c r="N24" s="33"/>
+      <c r="O24" s="33"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="25"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="27"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="42"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="52"/>
-      <c r="M25" s="52"/>
-      <c r="N25" s="39"/>
-      <c r="O25" s="40"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="51"/>
+      <c r="M25" s="51"/>
+      <c r="N25" s="27"/>
+      <c r="O25" s="28"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="38"/>
+      <c r="H26" s="26"/>
       <c r="I26" s="3"/>
       <c r="J26" s="10"/>
       <c r="K26" s="11"/>
-      <c r="L26" s="52"/>
-      <c r="M26" s="52"/>
+      <c r="L26" s="51"/>
+      <c r="M26" s="51"/>
       <c r="N26" s="12"/>
       <c r="O26" s="12"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
+      <c r="A27" s="35"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="52"/>
-      <c r="M27" s="52"/>
-      <c r="N27" s="45"/>
-      <c r="O27" s="45"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="51"/>
+      <c r="M27" s="51"/>
+      <c r="N27" s="33"/>
+      <c r="O27" s="33"/>
       <c r="S27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="41"/>
-      <c r="K28" s="41"/>
-      <c r="L28" s="52"/>
-      <c r="M28" s="52"/>
-      <c r="N28" s="43"/>
-      <c r="O28" s="40"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="51"/>
+      <c r="M28" s="51"/>
+      <c r="N28" s="31"/>
+      <c r="O28" s="28"/>
       <c r="S28" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
       <c r="E29" s="2"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -1409,86 +1406,89 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="4"/>
-      <c r="L29" s="52"/>
-      <c r="M29" s="52"/>
+      <c r="L29" s="51"/>
+      <c r="M29" s="51"/>
       <c r="N29" s="12"/>
       <c r="O29" s="2"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="54" t="s">
+      <c r="A30" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
       <c r="E30" s="2"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="52"/>
-      <c r="M30" s="52"/>
-      <c r="N30" s="43"/>
-      <c r="O30" s="40"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="51"/>
+      <c r="M30" s="51"/>
+      <c r="N30" s="31"/>
+      <c r="O30" s="28"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="54" t="s">
+      <c r="A31" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="54"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
       <c r="E31" s="2"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38"/>
-      <c r="K31" s="38"/>
-      <c r="L31" s="52"/>
-      <c r="M31" s="52"/>
-      <c r="N31" s="43"/>
-      <c r="O31" s="40"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="51"/>
+      <c r="M31" s="51"/>
+      <c r="N31" s="31"/>
+      <c r="O31" s="28"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="54" t="s">
+      <c r="A32" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="53"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="38"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="26"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
-      <c r="H32" s="38"/>
-      <c r="I32" s="38"/>
-      <c r="J32" s="38"/>
-      <c r="K32" s="38"/>
-      <c r="L32" s="52"/>
-      <c r="M32" s="52"/>
-      <c r="N32" s="39"/>
-      <c r="O32" s="40"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="51"/>
+      <c r="M32" s="51"/>
+      <c r="N32" s="27"/>
+      <c r="O32" s="28"/>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A33" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" s="50"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="38"/>
+      <c r="A33" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="44"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="26"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="4"/>
-      <c r="L33" s="52"/>
-      <c r="M33" s="52"/>
+      <c r="L33" s="51"/>
+      <c r="M33" s="51"/>
       <c r="N33" s="12"/>
-      <c r="O33" s="40"/>
+      <c r="O33" s="28"/>
+      <c r="S33" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
@@ -1498,20 +1498,20 @@
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C36" s="5"/>
-      <c r="D36" s="18" t="s">
+      <c r="D36" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E36" s="18"/>
+      <c r="E36" s="37"/>
       <c r="F36" s="6"/>
-      <c r="G36" s="18" t="s">
+      <c r="G36" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="H36" s="18"/>
+      <c r="H36" s="37"/>
       <c r="I36" s="7"/>
-      <c r="J36" s="18" t="s">
+      <c r="J36" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="K36" s="18"/>
+      <c r="K36" s="37"/>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="S39" t="s">
@@ -1519,13 +1519,13 @@
       </c>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
@@ -1535,324 +1535,324 @@
       <c r="E43" s="8"/>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B45" s="22" t="s">
+      <c r="B45" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="23"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="23"/>
-      <c r="G45" s="24"/>
-      <c r="J45" s="22" t="s">
+      <c r="C45" s="49"/>
+      <c r="D45" s="49"/>
+      <c r="E45" s="49"/>
+      <c r="F45" s="49"/>
+      <c r="G45" s="50"/>
+      <c r="J45" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="K45" s="23"/>
-      <c r="L45" s="23"/>
-      <c r="M45" s="23"/>
-      <c r="N45" s="23"/>
-      <c r="O45" s="24"/>
+      <c r="K45" s="49"/>
+      <c r="L45" s="49"/>
+      <c r="M45" s="49"/>
+      <c r="N45" s="49"/>
+      <c r="O45" s="50"/>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B46" s="25" t="s">
+      <c r="B46" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="27"/>
-      <c r="J46" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="K46" s="26"/>
-      <c r="L46" s="26"/>
-      <c r="M46" s="26"/>
-      <c r="N46" s="26"/>
-      <c r="O46" s="27"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="41"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="41"/>
+      <c r="G46" s="42"/>
+      <c r="J46" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="K46" s="41"/>
+      <c r="L46" s="41"/>
+      <c r="M46" s="41"/>
+      <c r="N46" s="41"/>
+      <c r="O46" s="42"/>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B47" s="25"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="27"/>
-      <c r="J47" s="25"/>
-      <c r="K47" s="26"/>
-      <c r="L47" s="26"/>
-      <c r="M47" s="26"/>
-      <c r="N47" s="26"/>
-      <c r="O47" s="27"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="42"/>
+      <c r="J47" s="40"/>
+      <c r="K47" s="41"/>
+      <c r="L47" s="41"/>
+      <c r="M47" s="41"/>
+      <c r="N47" s="41"/>
+      <c r="O47" s="42"/>
       <c r="W47" s="13"/>
       <c r="X47" s="13"/>
       <c r="Y47" s="13"/>
       <c r="Z47" s="13"/>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B48" s="25"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="27"/>
-      <c r="J48" s="25"/>
-      <c r="K48" s="26"/>
-      <c r="L48" s="26"/>
-      <c r="M48" s="26"/>
-      <c r="N48" s="26"/>
-      <c r="O48" s="27"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="41"/>
+      <c r="E48" s="41"/>
+      <c r="F48" s="41"/>
+      <c r="G48" s="42"/>
+      <c r="J48" s="40"/>
+      <c r="K48" s="41"/>
+      <c r="L48" s="41"/>
+      <c r="M48" s="41"/>
+      <c r="N48" s="41"/>
+      <c r="O48" s="42"/>
       <c r="W48" s="14"/>
       <c r="X48" s="14"/>
       <c r="Y48" s="14"/>
       <c r="Z48" s="14"/>
     </row>
     <row r="49" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B49" s="25"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="27"/>
-      <c r="J49" s="25"/>
-      <c r="K49" s="26"/>
-      <c r="L49" s="26"/>
-      <c r="M49" s="26"/>
-      <c r="N49" s="26"/>
-      <c r="O49" s="27"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="41"/>
+      <c r="G49" s="42"/>
+      <c r="J49" s="40"/>
+      <c r="K49" s="41"/>
+      <c r="L49" s="41"/>
+      <c r="M49" s="41"/>
+      <c r="N49" s="41"/>
+      <c r="O49" s="42"/>
       <c r="W49" s="14"/>
       <c r="X49" s="14"/>
       <c r="Y49" s="14"/>
       <c r="Z49" s="14"/>
     </row>
     <row r="50" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B50" s="25"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="27"/>
-      <c r="J50" s="25"/>
-      <c r="K50" s="26"/>
-      <c r="L50" s="26"/>
-      <c r="M50" s="26"/>
-      <c r="N50" s="26"/>
-      <c r="O50" s="27"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="41"/>
+      <c r="G50" s="42"/>
+      <c r="J50" s="40"/>
+      <c r="K50" s="41"/>
+      <c r="L50" s="41"/>
+      <c r="M50" s="41"/>
+      <c r="N50" s="41"/>
+      <c r="O50" s="42"/>
       <c r="W50" s="14"/>
       <c r="X50" s="14"/>
       <c r="Y50" s="14"/>
       <c r="Z50" s="14"/>
     </row>
     <row r="51" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B51" s="25"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="27"/>
-      <c r="J51" s="25"/>
-      <c r="K51" s="26"/>
-      <c r="L51" s="26"/>
-      <c r="M51" s="26"/>
-      <c r="N51" s="26"/>
-      <c r="O51" s="27"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="41"/>
+      <c r="D51" s="41"/>
+      <c r="E51" s="41"/>
+      <c r="F51" s="41"/>
+      <c r="G51" s="42"/>
+      <c r="J51" s="40"/>
+      <c r="K51" s="41"/>
+      <c r="L51" s="41"/>
+      <c r="M51" s="41"/>
+      <c r="N51" s="41"/>
+      <c r="O51" s="42"/>
       <c r="W51" s="14"/>
       <c r="X51" s="14"/>
       <c r="Y51" s="14"/>
       <c r="Z51" s="14"/>
     </row>
     <row r="52" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B52" s="25"/>
-      <c r="C52" s="26"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="26"/>
-      <c r="F52" s="26"/>
-      <c r="G52" s="27"/>
-      <c r="J52" s="25"/>
-      <c r="K52" s="26"/>
-      <c r="L52" s="26"/>
-      <c r="M52" s="26"/>
-      <c r="N52" s="26"/>
-      <c r="O52" s="27"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="41"/>
+      <c r="D52" s="41"/>
+      <c r="E52" s="41"/>
+      <c r="F52" s="41"/>
+      <c r="G52" s="42"/>
+      <c r="J52" s="40"/>
+      <c r="K52" s="41"/>
+      <c r="L52" s="41"/>
+      <c r="M52" s="41"/>
+      <c r="N52" s="41"/>
+      <c r="O52" s="42"/>
       <c r="W52" s="14"/>
       <c r="X52" s="14"/>
       <c r="Y52" s="14"/>
       <c r="Z52" s="14"/>
     </row>
     <row r="53" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B53" s="25"/>
-      <c r="C53" s="26"/>
-      <c r="D53" s="26"/>
-      <c r="E53" s="26"/>
-      <c r="F53" s="26"/>
-      <c r="G53" s="27"/>
-      <c r="J53" s="25"/>
-      <c r="K53" s="26"/>
-      <c r="L53" s="26"/>
-      <c r="M53" s="26"/>
-      <c r="N53" s="26"/>
-      <c r="O53" s="27"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="41"/>
+      <c r="D53" s="41"/>
+      <c r="E53" s="41"/>
+      <c r="F53" s="41"/>
+      <c r="G53" s="42"/>
+      <c r="J53" s="40"/>
+      <c r="K53" s="41"/>
+      <c r="L53" s="41"/>
+      <c r="M53" s="41"/>
+      <c r="N53" s="41"/>
+      <c r="O53" s="42"/>
       <c r="W53" s="13"/>
       <c r="X53" s="13"/>
       <c r="Y53" s="13"/>
       <c r="Z53" s="13"/>
     </row>
     <row r="54" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B54" s="25"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="26"/>
-      <c r="F54" s="26"/>
-      <c r="G54" s="27"/>
-      <c r="J54" s="25"/>
-      <c r="K54" s="26"/>
-      <c r="L54" s="26"/>
-      <c r="M54" s="26"/>
-      <c r="N54" s="26"/>
-      <c r="O54" s="27"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="41"/>
+      <c r="D54" s="41"/>
+      <c r="E54" s="41"/>
+      <c r="F54" s="41"/>
+      <c r="G54" s="42"/>
+      <c r="J54" s="40"/>
+      <c r="K54" s="41"/>
+      <c r="L54" s="41"/>
+      <c r="M54" s="41"/>
+      <c r="N54" s="41"/>
+      <c r="O54" s="42"/>
       <c r="W54" s="14"/>
       <c r="X54" s="14"/>
       <c r="Y54" s="14"/>
       <c r="Z54" s="14"/>
     </row>
     <row r="55" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B55" s="25"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26"/>
-      <c r="F55" s="26"/>
-      <c r="G55" s="27"/>
-      <c r="J55" s="25"/>
-      <c r="K55" s="26"/>
-      <c r="L55" s="26"/>
-      <c r="M55" s="26"/>
-      <c r="N55" s="26"/>
-      <c r="O55" s="27"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="41"/>
+      <c r="D55" s="41"/>
+      <c r="E55" s="41"/>
+      <c r="F55" s="41"/>
+      <c r="G55" s="42"/>
+      <c r="J55" s="40"/>
+      <c r="K55" s="41"/>
+      <c r="L55" s="41"/>
+      <c r="M55" s="41"/>
+      <c r="N55" s="41"/>
+      <c r="O55" s="42"/>
       <c r="W55" s="14"/>
       <c r="X55" s="14"/>
       <c r="Y55" s="14"/>
       <c r="Z55" s="14"/>
     </row>
     <row r="56" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B56" s="25"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
-      <c r="F56" s="26"/>
-      <c r="G56" s="27"/>
-      <c r="J56" s="25"/>
-      <c r="K56" s="26"/>
-      <c r="L56" s="26"/>
-      <c r="M56" s="26"/>
-      <c r="N56" s="26"/>
-      <c r="O56" s="27"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="41"/>
+      <c r="D56" s="41"/>
+      <c r="E56" s="41"/>
+      <c r="F56" s="41"/>
+      <c r="G56" s="42"/>
+      <c r="J56" s="40"/>
+      <c r="K56" s="41"/>
+      <c r="L56" s="41"/>
+      <c r="M56" s="41"/>
+      <c r="N56" s="41"/>
+      <c r="O56" s="42"/>
       <c r="W56" s="13"/>
       <c r="X56" s="13"/>
       <c r="Y56" s="13"/>
       <c r="Z56" s="13"/>
     </row>
     <row r="57" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B57" s="25"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="26"/>
-      <c r="F57" s="26"/>
-      <c r="G57" s="27"/>
-      <c r="J57" s="25"/>
-      <c r="K57" s="26"/>
-      <c r="L57" s="26"/>
-      <c r="M57" s="26"/>
-      <c r="N57" s="26"/>
-      <c r="O57" s="27"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="41"/>
+      <c r="D57" s="41"/>
+      <c r="E57" s="41"/>
+      <c r="F57" s="41"/>
+      <c r="G57" s="42"/>
+      <c r="J57" s="40"/>
+      <c r="K57" s="41"/>
+      <c r="L57" s="41"/>
+      <c r="M57" s="41"/>
+      <c r="N57" s="41"/>
+      <c r="O57" s="42"/>
       <c r="W57" s="13"/>
       <c r="X57" s="13"/>
       <c r="Y57" s="13"/>
       <c r="Z57" s="13"/>
     </row>
     <row r="58" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B58" s="25"/>
-      <c r="C58" s="26"/>
-      <c r="D58" s="26"/>
-      <c r="E58" s="26"/>
-      <c r="F58" s="26"/>
-      <c r="G58" s="27"/>
-      <c r="J58" s="25"/>
-      <c r="K58" s="26"/>
-      <c r="L58" s="26"/>
-      <c r="M58" s="26"/>
-      <c r="N58" s="26"/>
-      <c r="O58" s="27"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="41"/>
+      <c r="D58" s="41"/>
+      <c r="E58" s="41"/>
+      <c r="F58" s="41"/>
+      <c r="G58" s="42"/>
+      <c r="J58" s="40"/>
+      <c r="K58" s="41"/>
+      <c r="L58" s="41"/>
+      <c r="M58" s="41"/>
+      <c r="N58" s="41"/>
+      <c r="O58" s="42"/>
       <c r="W58" s="13"/>
       <c r="X58" s="13"/>
       <c r="Y58" s="13"/>
       <c r="Z58" s="13"/>
     </row>
     <row r="59" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B59" s="25"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="26"/>
-      <c r="E59" s="26"/>
-      <c r="F59" s="26"/>
-      <c r="G59" s="27"/>
-      <c r="J59" s="25"/>
-      <c r="K59" s="26"/>
-      <c r="L59" s="26"/>
-      <c r="M59" s="26"/>
-      <c r="N59" s="26"/>
-      <c r="O59" s="27"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="41"/>
+      <c r="D59" s="41"/>
+      <c r="E59" s="41"/>
+      <c r="F59" s="41"/>
+      <c r="G59" s="42"/>
+      <c r="J59" s="40"/>
+      <c r="K59" s="41"/>
+      <c r="L59" s="41"/>
+      <c r="M59" s="41"/>
+      <c r="N59" s="41"/>
+      <c r="O59" s="42"/>
       <c r="W59" s="13"/>
       <c r="X59" s="13"/>
       <c r="Y59" s="13"/>
       <c r="Z59" s="13"/>
     </row>
     <row r="60" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B60" s="25"/>
-      <c r="C60" s="26"/>
-      <c r="D60" s="26"/>
-      <c r="E60" s="26"/>
-      <c r="F60" s="26"/>
-      <c r="G60" s="27"/>
-      <c r="J60" s="25"/>
-      <c r="K60" s="26"/>
-      <c r="L60" s="26"/>
-      <c r="M60" s="26"/>
-      <c r="N60" s="26"/>
-      <c r="O60" s="27"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="41"/>
+      <c r="D60" s="41"/>
+      <c r="E60" s="41"/>
+      <c r="F60" s="41"/>
+      <c r="G60" s="42"/>
+      <c r="J60" s="40"/>
+      <c r="K60" s="41"/>
+      <c r="L60" s="41"/>
+      <c r="M60" s="41"/>
+      <c r="N60" s="41"/>
+      <c r="O60" s="42"/>
       <c r="W60" s="13"/>
       <c r="X60" s="13"/>
       <c r="Y60" s="13"/>
       <c r="Z60" s="13"/>
     </row>
     <row r="61" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B61" s="25"/>
-      <c r="C61" s="26"/>
-      <c r="D61" s="26"/>
-      <c r="E61" s="26"/>
-      <c r="F61" s="26"/>
-      <c r="G61" s="27"/>
-      <c r="J61" s="25"/>
-      <c r="K61" s="26"/>
-      <c r="L61" s="26"/>
-      <c r="M61" s="26"/>
-      <c r="N61" s="26"/>
-      <c r="O61" s="27"/>
+      <c r="B61" s="40"/>
+      <c r="C61" s="41"/>
+      <c r="D61" s="41"/>
+      <c r="E61" s="41"/>
+      <c r="F61" s="41"/>
+      <c r="G61" s="42"/>
+      <c r="J61" s="40"/>
+      <c r="K61" s="41"/>
+      <c r="L61" s="41"/>
+      <c r="M61" s="41"/>
+      <c r="N61" s="41"/>
+      <c r="O61" s="42"/>
       <c r="W61" s="13"/>
       <c r="X61" s="13"/>
       <c r="Y61" s="13"/>
       <c r="Z61" s="13"/>
     </row>
     <row r="62" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B62" s="25"/>
-      <c r="C62" s="26"/>
-      <c r="D62" s="26"/>
-      <c r="E62" s="26"/>
-      <c r="F62" s="26"/>
-      <c r="G62" s="27"/>
-      <c r="J62" s="25"/>
-      <c r="K62" s="26"/>
-      <c r="L62" s="26"/>
-      <c r="M62" s="26"/>
-      <c r="N62" s="26"/>
-      <c r="O62" s="27"/>
+      <c r="B62" s="40"/>
+      <c r="C62" s="41"/>
+      <c r="D62" s="41"/>
+      <c r="E62" s="41"/>
+      <c r="F62" s="41"/>
+      <c r="G62" s="42"/>
+      <c r="J62" s="40"/>
+      <c r="K62" s="41"/>
+      <c r="L62" s="41"/>
+      <c r="M62" s="41"/>
+      <c r="N62" s="41"/>
+      <c r="O62" s="42"/>
       <c r="W62" s="15"/>
       <c r="X62" s="13"/>
       <c r="Y62" s="13"/>
@@ -1872,13 +1872,6 @@
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="L6:M33"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A12:D12"/>
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="A30:D30"/>
     <mergeCell ref="A31:D31"/>
@@ -1887,6 +1880,7 @@
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A21:D21"/>
     <mergeCell ref="J62:O62"/>
     <mergeCell ref="B60:G60"/>
     <mergeCell ref="B61:G61"/>
@@ -1911,7 +1905,6 @@
     <mergeCell ref="B53:G53"/>
     <mergeCell ref="B54:G54"/>
     <mergeCell ref="B55:G55"/>
-    <mergeCell ref="A1:E1"/>
     <mergeCell ref="J50:O50"/>
     <mergeCell ref="A32:D32"/>
     <mergeCell ref="J36:K36"/>
@@ -1927,8 +1920,7 @@
     <mergeCell ref="B46:G46"/>
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="B48:G48"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="L6:M33"/>
     <mergeCell ref="A42:E42"/>
     <mergeCell ref="A29:D29"/>
     <mergeCell ref="A22:D22"/>
@@ -1940,12 +1932,20 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A1:E1"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A12:D12"/>
   </mergeCells>
   <conditionalFormatting sqref="I22:J22">
     <cfRule type="colorScale" priority="46">

</xml_diff>